<commit_message>
Cambio etiquetas datos Excel
</commit_message>
<xml_diff>
--- a/datos-exportados-plantilla.xlsx
+++ b/datos-exportados-plantilla.xlsx
@@ -29,12 +29,18 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="4">
   <si>
     <t xml:space="preserve">Años</t>
   </si>
   <si>
     <t xml:space="preserve">Corridas</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Año</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Corrida</t>
   </si>
 </sst>
 </file>
@@ -168,7 +174,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:L32"/>
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -729,7 +735,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1:L32"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -738,7 +744,7 @@
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="5" t="s">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="D1" s="5"/>
       <c r="E1" s="5"/>
@@ -786,7 +792,7 @@
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="5" t="s">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="B3" s="3" t="n">
         <v>1</v>
@@ -1290,7 +1296,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="A1:L32"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1851,7 +1857,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="A1:L32"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2412,7 +2418,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="A1:L32"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -2973,7 +2979,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="A1:L32"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3534,7 +3540,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="A1:L32"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4095,7 +4101,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="A1:L32"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -4656,7 +4662,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="A1:L32"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -5217,7 +5223,7 @@
   <dimension ref="A1:L32"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="A1:L32"/>
+      <selection pane="topLeft" activeCell="I15" activeCellId="0" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>

</xml_diff>